<commit_message>
Add Get Excel Cells script
</commit_message>
<xml_diff>
--- a/files/tests/pattern.xlsx
+++ b/files/tests/pattern.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="My List" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
   <si>
     <t>User“s registration information</t>
   </si>
@@ -40,13 +41,16 @@
   </si>
   <si>
     <t>#usr.company#</t>
+  </si>
+  <si>
+    <t>#usr.id# - #usr.name#</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -63,6 +67,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="2">
@@ -85,10 +96,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -392,9 +404,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -440,4 +450,39 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Обычный"&amp;12Страница &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="27.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>